<commit_message>
add : .gitignore 파일 추가
</commit_message>
<xml_diff>
--- a/webtoon_review.xlsx
+++ b/webtoon_review.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruheekim/Desktop/EWHA/2021-1학기/웹과 텍스트마이닝개론/웹텍마 기말 프로젝트/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{096528CF-6E67-B848-BD4D-FFB46C54C77F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{468EEA64-7892-414E-96C7-FE30AB33225E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16220" xr2:uid="{A3C87630-6A14-CE48-96C6-ADFDF98FFF43}"/>
   </bookViews>
@@ -1456,8 +1456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D837047-7676-FA46-AFA2-B5D08CD4C602}">
   <dimension ref="A1:B420"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="C60" sqref="C60"/>
+    <sheetView tabSelected="1" topLeftCell="A397" workbookViewId="0">
+      <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>